<commit_message>
Tried to create some visualizations
</commit_message>
<xml_diff>
--- a/data/rainfall-temp-roanke-monthly.xlsx
+++ b/data/rainfall-temp-roanke-monthly.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julierebstock/Desktop/Virginia-Tech/DSPG-2021/Floyd-County/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julierebstock/Desktop/Virginia-Tech/DSPG-2021/Floyd-County/DSPG_Floyd/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B9DC721-CB70-5D46-8DC1-062F5D082959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F92E924A-4EF2-9140-BEB3-FF06DE80C41F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{908A36FC-4A53-5445-AE53-455C6005B6D6}"/>
   </bookViews>
@@ -42,49 +42,49 @@
     <t xml:space="preserve">Month </t>
   </si>
   <si>
-    <t xml:space="preserve">Wind Max </t>
-  </si>
-  <si>
-    <t xml:space="preserve">January </t>
-  </si>
-  <si>
-    <t>February</t>
-  </si>
-  <si>
-    <t>March</t>
-  </si>
-  <si>
-    <t>April</t>
-  </si>
-  <si>
     <t xml:space="preserve">May </t>
   </si>
   <si>
-    <t>June</t>
-  </si>
-  <si>
-    <t>July</t>
-  </si>
-  <si>
-    <t>August</t>
-  </si>
-  <si>
-    <t>September</t>
-  </si>
-  <si>
-    <t>October</t>
-  </si>
-  <si>
-    <t xml:space="preserve">November </t>
-  </si>
-  <si>
-    <t xml:space="preserve">December </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Average Temp (F) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Average Rainfall (inches) </t>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>Feb</t>
+  </si>
+  <si>
+    <t>Mar</t>
+  </si>
+  <si>
+    <t>Apr</t>
+  </si>
+  <si>
+    <t>Jun</t>
+  </si>
+  <si>
+    <t>Jul</t>
+  </si>
+  <si>
+    <t>Aug</t>
+  </si>
+  <si>
+    <t>Sep</t>
+  </si>
+  <si>
+    <t>Oct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nov </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dec </t>
+  </si>
+  <si>
+    <t>Average_Temp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wind_Max </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average_Rainfall </t>
   </si>
 </sst>
 </file>
@@ -439,7 +439,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="212" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -459,10 +459,10 @@
         <v>16</v>
       </c>
       <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
         <v>15</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -538,7 +538,7 @@
         <v>2017</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C6">
         <v>0.26</v>
@@ -555,7 +555,7 @@
         <v>2017</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7">
         <v>0.15</v>
@@ -572,7 +572,7 @@
         <v>2017</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8">
         <v>7.0000000000000007E-2</v>
@@ -589,7 +589,7 @@
         <v>2017</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9">
         <v>7.0000000000000007E-2</v>
@@ -606,7 +606,7 @@
         <v>2017</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10">
         <v>0.08</v>
@@ -623,7 +623,7 @@
         <v>2017</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11">
         <v>0.13</v>
@@ -640,7 +640,7 @@
         <v>2017</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12">
         <v>0.02</v>
@@ -657,7 +657,7 @@
         <v>2017</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13">
         <v>0.01</v>

</xml_diff>